<commit_message>
LI added D53 sect. 2
</commit_message>
<xml_diff>
--- a/doc/COACHES_deliverables.xlsx
+++ b/doc/COACHES_deliverables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="1455" yWindow="270" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -123,42 +123,12 @@
     <t>VUB</t>
   </si>
   <si>
-    <t>D3.1.1</t>
-  </si>
-  <si>
-    <t>D3.1.2</t>
-  </si>
-  <si>
-    <t>D3.2.1</t>
-  </si>
-  <si>
-    <t>D3.2.2</t>
-  </si>
-  <si>
     <t>Multi-modal human-robot interaction</t>
   </si>
   <si>
     <t>Human needs estimation</t>
   </si>
   <si>
-    <t>Developed software for multi-modal human-robot interaction</t>
-  </si>
-  <si>
-    <t>Developed software for human needs estimation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Document of specification of localisation and navigation methods </t>
-  </si>
-  <si>
-    <t>A software of navigation module to integrate in the whole architecture</t>
-  </si>
-  <si>
-    <t>Document of specification of multi-robot planning using DEC-POMDP</t>
-  </si>
-  <si>
-    <t>A software of decision module to integrate in the whole architecture</t>
-  </si>
-  <si>
     <t xml:space="preserve">Description and specification of the proposed solutions for the sensor processing </t>
   </si>
   <si>
@@ -193,6 +163,36 @@
   </si>
   <si>
     <t>Draft</t>
+  </si>
+  <si>
+    <t>D3.1</t>
+  </si>
+  <si>
+    <t>D3.2</t>
+  </si>
+  <si>
+    <t>D3.3</t>
+  </si>
+  <si>
+    <t>D3.4</t>
+  </si>
+  <si>
+    <t>Software component for human needs estimation</t>
+  </si>
+  <si>
+    <t>Software component for multi-modal human-robot interaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specification of localisation and navigation methods </t>
+  </si>
+  <si>
+    <t>Software component for navigation</t>
+  </si>
+  <si>
+    <t>Specification of decision making and multi-robot planning</t>
+  </si>
+  <si>
+    <t>Software component for decision making and multi-robot planning</t>
   </si>
 </sst>
 </file>
@@ -334,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -398,6 +398,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -702,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,7 +732,7 @@
         <v>23</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -746,7 +749,7 @@
         <v>24</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -763,7 +766,7 @@
         <v>25</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -774,10 +777,10 @@
         <v>12</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E4" s="18"/>
     </row>
@@ -792,7 +795,7 @@
         <v>26</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E5" s="18"/>
     </row>
@@ -819,13 +822,13 @@
         <v>18</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -836,7 +839,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>30</v>
@@ -854,7 +857,7 @@
         <v>34</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E9" s="18"/>
     </row>
@@ -869,7 +872,7 @@
         <v>34</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E10" s="18"/>
     </row>
@@ -914,7 +917,7 @@
         <v>34</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E13" s="18"/>
     </row>
@@ -929,7 +932,7 @@
         <v>34</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E14" s="18"/>
     </row>
@@ -941,10 +944,10 @@
         <v>24</v>
       </c>
       <c r="C15" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>55</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>43</v>
       </c>
       <c r="E15" s="18"/>
     </row>
@@ -956,61 +959,61 @@
         <v>24</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E16" s="18"/>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="10">
+        <v>21</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>35</v>
-      </c>
-      <c r="B17" s="10">
-        <v>27</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>39</v>
       </c>
       <c r="E17" s="18"/>
     </row>
     <row r="18" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B18" s="10">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E18" s="18"/>
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B19" s="10">
         <v>27</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E19" s="18"/>
     </row>
     <row r="20" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B20" s="10">
         <v>27</v>
@@ -1019,7 +1022,7 @@
         <v>26</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E20" s="18"/>
     </row>
@@ -1034,10 +1037,10 @@
         <v>26</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1050,8 +1053,8 @@
       <c r="C22" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="12" t="s">
-        <v>46</v>
+      <c r="D22" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="E22" s="18"/>
     </row>
@@ -1066,7 +1069,7 @@
         <v>26</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E23" s="18"/>
     </row>
@@ -1093,10 +1096,10 @@
         <v>36</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E25" s="19"/>
     </row>

</xml_diff>